<commit_message>
add sending mail template util and modfity make letter
</commit_message>
<xml_diff>
--- a/data/activities/follower.xlsx
+++ b/data/activities/follower.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\activity_management\data\activities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6D7838-CFBE-494D-90C0-504A725F95D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB74436-EFB7-4EBD-9288-F1F15D00A438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,16 @@
     <sheet name="報名名單" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>報名時間</t>
   </si>
@@ -119,33 +124,6 @@
   </si>
   <si>
     <t>其他</t>
-  </si>
-  <si>
-    <t>2025-02-27 16:38:02</t>
-  </si>
-  <si>
-    <t>20250227A217506</t>
-  </si>
-  <si>
-    <t>李如琪</t>
-  </si>
-  <si>
-    <t>奇美醫院臨床試驗中心</t>
-  </si>
-  <si>
-    <t>小組長</t>
-  </si>
-  <si>
-    <t>06-2812811轉57267</t>
-  </si>
-  <si>
-    <t>0988301381</t>
-  </si>
-  <si>
-    <t>D220225670</t>
-  </si>
-  <si>
-    <t>是</t>
   </si>
   <si>
     <t>tanyayu@mpat.org.tw</t>
@@ -542,17 +520,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDD35E17-AB28-48A4-B14A-5998ABDF408A}">
-  <dimension ref="A1:AI4"/>
+  <dimension ref="A1:AI3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -561,7 +539,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -579,7 +557,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>7</v>
@@ -648,7 +626,7 @@
       </c>
       <c r="I2" s="2"/>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>21</v>
@@ -713,7 +691,7 @@
       </c>
       <c r="I3" s="2"/>
       <c r="J3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>21</v>
@@ -751,73 +729,6 @@
       <c r="AH3" s="2"/>
       <c r="AI3" s="2"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="2"/>
-      <c r="AG4" s="2"/>
-      <c r="AH4" s="2"/>
-      <c r="AI4" s="2"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>